<commit_message>
latest updated Files after conflicts
</commit_message>
<xml_diff>
--- a/filesToUpload/EmailTemplate.xlsx
+++ b/filesToUpload/EmailTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wasim\git\DACAutomation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wasim\git\DACAutomation\filesToUpload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5231D487-F688-4F18-9C5A-2E19079F710D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB69A176-DB08-44E0-9A5D-2CEC040CE524}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16920" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -475,15 +475,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -509,12 +509,6 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -529,7 +523,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>